<commit_message>
add readme, delete wsc, check inventory
</commit_message>
<xml_diff>
--- a/AF4_conf.xlsx
+++ b/AF4_conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PTWork\SCRIPTS\ptaf-pro-conf_ansible-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C2448A-0EF8-46F3-A961-C1C90D0EFC99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E92204-E0E2-41FC-8696-780CAAFFD9D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10185" windowHeight="11745" xr2:uid="{BDDD9177-F6CF-42C1-B99E-562E59E75EA2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="758">
   <si>
     <t>DNS сервера</t>
   </si>
@@ -2137,45 +2137,174 @@
     <t>time.google.com</t>
   </si>
   <si>
+    <t>ptaf-vm1</t>
+  </si>
+  <si>
+    <t>P@ssw0rd</t>
+  </si>
+  <si>
+    <t>bond0_mode</t>
+  </si>
+  <si>
+    <t>Grafana (VIP-ы не должны быть в CLUSTER подсети)</t>
+  </si>
+  <si>
+    <t>UI (VIP-ы не должны быть в CLUSTER подсети)</t>
+  </si>
+  <si>
+    <t>Подключение агентов (VIP-ы не должны быть в CLUSTER подсети)</t>
+  </si>
+  <si>
+    <t>bond1_mode</t>
+  </si>
+  <si>
+    <t>bond2_mode</t>
+  </si>
+  <si>
+    <t>bond3_mode</t>
+  </si>
+  <si>
+    <t>Тэг vlan1</t>
+  </si>
+  <si>
+    <t>Тэг vlan2</t>
+  </si>
+  <si>
+    <t>Тэг vlan3</t>
+  </si>
+  <si>
+    <t>Тэг vlan4</t>
+  </si>
+  <si>
+    <t>bond0_int1</t>
+  </si>
+  <si>
+    <t>bond0_int2</t>
+  </si>
+  <si>
+    <t>bond0 интерфейс1</t>
+  </si>
+  <si>
+    <t>bond0 интерфейс2</t>
+  </si>
+  <si>
+    <t>bond1_int1</t>
+  </si>
+  <si>
+    <t>bond1_int2</t>
+  </si>
+  <si>
+    <t>bond1 интерфейс1</t>
+  </si>
+  <si>
+    <t>bond2_int1</t>
+  </si>
+  <si>
+    <t>bond2_int2</t>
+  </si>
+  <si>
+    <t>bond3_int1</t>
+  </si>
+  <si>
+    <t>bond3_int2</t>
+  </si>
+  <si>
+    <t>bond0_tag1</t>
+  </si>
+  <si>
+    <t>bond0_tag2</t>
+  </si>
+  <si>
+    <t>bond0_tag3</t>
+  </si>
+  <si>
+    <t>bond0_tag4</t>
+  </si>
+  <si>
+    <t>bond1_tag1</t>
+  </si>
+  <si>
+    <t>bond1_tag2</t>
+  </si>
+  <si>
+    <t>bond1_tag3</t>
+  </si>
+  <si>
+    <t>bond1_tag4</t>
+  </si>
+  <si>
+    <t>bond2_tag1</t>
+  </si>
+  <si>
+    <t>bond2_tag2</t>
+  </si>
+  <si>
+    <t>bond2_tag3</t>
+  </si>
+  <si>
+    <t>bond2_tag4</t>
+  </si>
+  <si>
+    <t>bond3_tag1</t>
+  </si>
+  <si>
+    <t>bond3_tag2</t>
+  </si>
+  <si>
+    <t>bond3_tag3</t>
+  </si>
+  <si>
+    <t>bond3_tag4</t>
+  </si>
+  <si>
+    <t>bond2 интерфейс1</t>
+  </si>
+  <si>
+    <t>bond3 интерфейс1</t>
+  </si>
+  <si>
+    <t>bond2 интерфейс2</t>
+  </si>
+  <si>
+    <t>bond3 интерфейс2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нужны бонды? </t>
+  </si>
+  <si>
+    <t>Режим бонда (0 — round-robin; 1 — active-backup); 2 — balance-xor; 3 — broadcast; 4 — 802.3ad; 5 — balance-tlb; 6 — balance-alb.)</t>
+  </si>
+  <si>
+    <t>bond1 интерфейс2</t>
+  </si>
+  <si>
+    <t>ptaf-vm2</t>
+  </si>
+  <si>
+    <t>ptaf-vm3</t>
+  </si>
+  <si>
+    <t>172.16.10.11</t>
+  </si>
+  <si>
+    <t>172.16.10.12</t>
+  </si>
+  <si>
+    <t>192.168.88.171</t>
+  </si>
+  <si>
+    <t>192.168.88.172</t>
+  </si>
+  <si>
+    <t>192.168.88.173</t>
+  </si>
+  <si>
+    <t>192.168.88.1</t>
+  </si>
+  <si>
     <t>8.8.8.8</t>
   </si>
   <si>
-    <t>172.16.10.11</t>
-  </si>
-  <si>
-    <t>172.16.10.12</t>
-  </si>
-  <si>
-    <t>ptaf-vm1</t>
-  </si>
-  <si>
-    <t>ptaf-vm2</t>
-  </si>
-  <si>
-    <t>ptaf-vm3</t>
-  </si>
-  <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
-    <t>192.168.88.171</t>
-  </si>
-  <si>
-    <t>192.168.88.172</t>
-  </si>
-  <si>
-    <t>192.168.88.173</t>
-  </si>
-  <si>
-    <t>192.168.88.1</t>
-  </si>
-  <si>
-    <t>P@ssw0rd</t>
-  </si>
-  <si>
     <t>192.168.88.170</t>
   </si>
   <si>
@@ -2183,147 +2312,6 @@
   </si>
   <si>
     <t>ens19</t>
-  </si>
-  <si>
-    <t>bond0_mode</t>
-  </si>
-  <si>
-    <t>Grafana (VIP-ы не должны быть в CLUSTER подсети)</t>
-  </si>
-  <si>
-    <t>UI (VIP-ы не должны быть в CLUSTER подсети)</t>
-  </si>
-  <si>
-    <t>Подключение агентов (VIP-ы не должны быть в CLUSTER подсети)</t>
-  </si>
-  <si>
-    <t>bond1_mode</t>
-  </si>
-  <si>
-    <t>bond2_mode</t>
-  </si>
-  <si>
-    <t>bond3_mode</t>
-  </si>
-  <si>
-    <t>Тэг vlan1</t>
-  </si>
-  <si>
-    <t>Тэг vlan2</t>
-  </si>
-  <si>
-    <t>Тэг vlan3</t>
-  </si>
-  <si>
-    <t>Тэг vlan4</t>
-  </si>
-  <si>
-    <t>bond0_int1</t>
-  </si>
-  <si>
-    <t>bond0_int2</t>
-  </si>
-  <si>
-    <t>bond0 интерфейс1</t>
-  </si>
-  <si>
-    <t>bond0 интерфейс2</t>
-  </si>
-  <si>
-    <t>bond1_int1</t>
-  </si>
-  <si>
-    <t>bond1_int2</t>
-  </si>
-  <si>
-    <t>bond1 интерфейс1</t>
-  </si>
-  <si>
-    <t>bond2_int1</t>
-  </si>
-  <si>
-    <t>bond2_int2</t>
-  </si>
-  <si>
-    <t>bond3_int1</t>
-  </si>
-  <si>
-    <t>bond3_int2</t>
-  </si>
-  <si>
-    <t>bond0_tag1</t>
-  </si>
-  <si>
-    <t>bond0_tag2</t>
-  </si>
-  <si>
-    <t>bond0_tag3</t>
-  </si>
-  <si>
-    <t>bond0_tag4</t>
-  </si>
-  <si>
-    <t>bond1_tag1</t>
-  </si>
-  <si>
-    <t>bond1_tag2</t>
-  </si>
-  <si>
-    <t>bond1_tag3</t>
-  </si>
-  <si>
-    <t>bond1_tag4</t>
-  </si>
-  <si>
-    <t>bond2_tag1</t>
-  </si>
-  <si>
-    <t>bond2_tag2</t>
-  </si>
-  <si>
-    <t>bond2_tag3</t>
-  </si>
-  <si>
-    <t>bond2_tag4</t>
-  </si>
-  <si>
-    <t>bond3_tag1</t>
-  </si>
-  <si>
-    <t>bond3_tag2</t>
-  </si>
-  <si>
-    <t>bond3_tag3</t>
-  </si>
-  <si>
-    <t>bond3_tag4</t>
-  </si>
-  <si>
-    <t>bond2 интерфейс1</t>
-  </si>
-  <si>
-    <t>bond3 интерфейс1</t>
-  </si>
-  <si>
-    <t>bond2 интерфейс2</t>
-  </si>
-  <si>
-    <t>bond3 интерфейс2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нужны бонды? </t>
-  </si>
-  <si>
-    <t>Режим бонда (0 — round-robin; 1 — active-backup); 2 — balance-xor; 3 — broadcast; 4 — 802.3ad; 5 — balance-tlb; 6 — balance-alb.)</t>
-  </si>
-  <si>
-    <t>bond1 интерфейс2</t>
-  </si>
-  <si>
-    <t>bond0</t>
-  </si>
-  <si>
-    <t>bond1</t>
   </si>
 </sst>
 </file>
@@ -2926,9 +2914,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCC04E1-6663-4A2B-96A2-6DC7EB085CB3}">
   <dimension ref="A1:AP594"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3065,13 +3053,13 @@
         <v>63</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>711</v>
+        <v>700</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -3103,13 +3091,13 @@
         <v>32</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>703</v>
+        <v>746</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>704</v>
+        <v>747</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -3141,13 +3129,13 @@
         <v>678</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>713</v>
+        <v>756</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -3175,13 +3163,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>707</v>
+        <v>750</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>708</v>
+        <v>751</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>709</v>
+        <v>752</v>
       </c>
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
@@ -3241,13 +3229,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>710</v>
+        <v>753</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>710</v>
+        <v>753</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>710</v>
+        <v>753</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
@@ -3344,13 +3332,13 @@
         <v>679</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>714</v>
+        <v>757</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>681</v>
+        <v>757</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -3380,10 +3368,10 @@
         <v>697</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>700</v>
+        <v>748</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>701</v>
+        <v>749</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -3992,14 +3980,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>699</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>705</v>
-      </c>
-      <c r="E33" s="37" t="s">
-        <v>706</v>
-      </c>
+        <v>754</v>
+      </c>
+      <c r="D33" s="36"/>
+      <c r="E33" s="37"/>
       <c r="AA33" t="s">
         <v>46</v>
       </c>
@@ -4012,13 +3996,13 @@
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>712</v>
+      <c r="C34" s="33" t="s">
+        <v>755</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -4038,13 +4022,13 @@
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>712</v>
+        <v>755</v>
       </c>
       <c r="D35" s="10"/>
       <c r="F35" s="26" t="str">
@@ -4057,13 +4041,13 @@
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>712</v>
+        <v>755</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -4112,7 +4096,7 @@
     </row>
     <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>694</v>
@@ -4129,10 +4113,10 @@
     </row>
     <row r="40" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="C40" s="39"/>
       <c r="D40" s="39"/>
@@ -4164,10 +4148,10 @@
     </row>
     <row r="41" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="C41" s="39"/>
       <c r="D41" s="39"/>
@@ -4196,10 +4180,10 @@
     </row>
     <row r="42" spans="1:42" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="C42" s="39"/>
       <c r="D42" s="39"/>
@@ -4231,10 +4215,10 @@
     </row>
     <row r="43" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
       <c r="C43" s="39"/>
       <c r="D43" s="39"/>
@@ -4266,10 +4250,10 @@
     </row>
     <row r="44" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="C44" s="39"/>
       <c r="D44" s="39"/>
@@ -4301,10 +4285,10 @@
     </row>
     <row r="45" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="C45" s="39"/>
       <c r="D45" s="39"/>
@@ -4336,10 +4320,10 @@
     </row>
     <row r="46" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="C46" s="39"/>
       <c r="D46" s="39"/>
@@ -4371,10 +4355,10 @@
     </row>
     <row r="47" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
@@ -4406,10 +4390,10 @@
     </row>
     <row r="48" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
@@ -4441,10 +4425,10 @@
     </row>
     <row r="49" spans="1:42" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="40"/>
@@ -4470,10 +4454,10 @@
     </row>
     <row r="50" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -4499,10 +4483,10 @@
     </row>
     <row r="51" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -4528,10 +4512,10 @@
     </row>
     <row r="52" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4557,10 +4541,10 @@
     </row>
     <row r="53" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
@@ -4586,10 +4570,10 @@
     </row>
     <row r="54" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="C54" s="39"/>
       <c r="D54" s="39"/>
@@ -4615,10 +4599,10 @@
     </row>
     <row r="55" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="39"/>
@@ -4644,10 +4628,10 @@
     </row>
     <row r="56" spans="1:42" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="C56" s="39"/>
       <c r="D56" s="39"/>
@@ -4673,10 +4657,10 @@
     </row>
     <row r="57" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="C57" s="39"/>
       <c r="D57" s="39"/>
@@ -4702,10 +4686,10 @@
     </row>
     <row r="58" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="C58" s="39"/>
       <c r="D58" s="39"/>
@@ -4731,10 +4715,10 @@
     </row>
     <row r="59" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="C59" s="39"/>
       <c r="D59" s="39"/>
@@ -4760,10 +4744,10 @@
     </row>
     <row r="60" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="C60" s="39"/>
       <c r="D60" s="39"/>
@@ -4789,10 +4773,10 @@
     </row>
     <row r="61" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40"/>
@@ -4818,10 +4802,10 @@
     </row>
     <row r="62" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="40"/>
@@ -4847,10 +4831,10 @@
     </row>
     <row r="63" spans="1:42" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40"/>
@@ -4876,10 +4860,10 @@
     </row>
     <row r="64" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
@@ -4905,10 +4889,10 @@
     </row>
     <row r="65" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="C65" s="40"/>
       <c r="D65" s="40"/>
@@ -4934,10 +4918,10 @@
     </row>
     <row r="66" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="C66" s="40"/>
       <c r="D66" s="40"/>
@@ -4963,10 +4947,10 @@
     </row>
     <row r="67" spans="1:42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
       <c r="C67" s="40"/>
       <c r="D67" s="40"/>
@@ -7631,16 +7615,16 @@
   </sortState>
   <dataConsolidate/>
   <dataValidations count="15">
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="IP address" error="Please enter correct IP address" sqref="D33:E33 Y12 Y14 Y6 C26:Y26 Y20 Y8 C20:T20 Y18 C24:Y24 C8:T8 C18:T18 C31:E31 C14:T14 C12:T12 C6:T6 C33:C36" xr:uid="{F4A9DD59-10E1-4570-A620-994D614F80F3}">
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="IP address" error="Please enter correct IP address" sqref="D33:E33 Y12 Y14 Y6 C26:Y26 Y20 Y8 C20:T20 Y18 C24:Y24 C12:T12 C18:T18 C31:E31 C14:T14 C6:T6 C8:T8 C33:C36" xr:uid="{F4A9DD59-10E1-4570-A620-994D614F80F3}">
       <formula1>AND(LEN(C6)-LEN(SUBSTITUTE(C6,".",""))=3,--LEFT(C6,FIND(".",C6)-1)&lt;224,--LEFT(C6,FIND(".",C6)-1)&gt;0,--MID(SUBSTITUTE(C6,".","    "),6,5)&lt;256,--MID(SUBSTITUTE(C6,".","      "),15,7)&lt;256,--MID(SUBSTITUTE(C6,".","      "),22,10)&lt;256)</formula1>
     </dataValidation>
     <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Netmask" error="Please enter correct netmask" sqref="Y7 C25:Y25 Y19 Y13 C7:T7 C19:T19 C13:T13" xr:uid="{A53661DA-36E4-4B74-A278-B7516EFEA0F7}">
       <formula1>AND(LEN(C7)-LEN(SUBSTITUTE(C7,".",""))=3,--LEFT(C7,FIND(".",C7)-1)&lt;256,--LEFT(C7,FIND(".",C7)-1)&gt;0,--MID(SUBSTITUTE(C7,".","    "),6,5)&lt;256,--MID(SUBSTITUTE(C7,".","      "),15,7)&lt;256,--MID(SUBSTITUTE(C7,".","      "),22,10)&lt;256)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9 C27:Y27 Y21 Y15 C21:T21 C15:T15 C9:T9" xr:uid="{DC81CD85-3F94-40CD-B28A-B7045572A454}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9 C27:Y27 Y21 Y15 C21:T21 C9:T9 C15:T15" xr:uid="{DC81CD85-3F94-40CD-B28A-B7045572A454}">
       <formula1>$AA$31:$AA$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y16:Y17 Y22:Y23 Y10:Y11 C28:Y28 C22:T22 C16:T16 C10:T10" xr:uid="{67254EA8-B30E-4C33-9A6E-E36F6614BE2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y16:Y17 Y22:Y23 Y10:Y11 C28:Y28 C22:T22 C10:T10 C16:T16" xr:uid="{67254EA8-B30E-4C33-9A6E-E36F6614BE2B}">
       <formula1>$AA$36:$AA$37</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C29:T29" xr:uid="{8F4CC75D-0DB7-447A-A061-870AE6B3FAB9}">
@@ -7678,12 +7662,11 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{75094916-C9E8-45BD-81BC-515462435568}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{C776F13A-B8A8-4E0B-92A7-412E45BCF637}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{151511E1-952D-4A9F-A2B7-5229FDB36300}"/>
+    <hyperlink ref="D3:E3" r:id="rId2" display="P@ssw0rd" xr:uid="{31D6CA04-2191-4E38-A33D-DAD2D726D26A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>